<commit_message>
updated to STM merge version
</commit_message>
<xml_diff>
--- a/Review_STM_Combined_Feeds_20200511.xlsx
+++ b/Review_STM_Combined_Feeds_20200511.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_WORK\00 Project\AEP\ODS\Nung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\AEP_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8CDA2E-CA2E-402E-8DF9-1477AC52BDA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF2258-C0D5-4ECD-8B0E-5B025CA1A5E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{280DBBAB-34EF-4FDD-92E3-7E03923A9C0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{280DBBAB-34EF-4FDD-92E3-7E03923A9C0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Comment</t>
   </si>
@@ -77,12 +77,33 @@
 DWO_PRM_REV_SHARE - CALLEDNUMBERMASTER
 DWO_PRM_REV_SHARE_POST - CALLEDNUMBERMASTER</t>
   </si>
+  <si>
+    <t>encrypt('66' || SERVICENUMBER)</t>
+  </si>
+  <si>
+    <t>CBS_TS_PRODPRICEPLN_DTN</t>
+  </si>
+  <si>
+    <t>DIM_CBS _TS_PRODPRICEPLN</t>
+  </si>
+  <si>
+    <t>CBS_PRODUCTEXTATTR_DTN</t>
+  </si>
+  <si>
+    <t>DIM_CBS_PRODUCTEXTATTR</t>
+  </si>
+  <si>
+    <t>CBS_USAGESERVICETPE_DTN</t>
+  </si>
+  <si>
+    <t>DIM_DEF_CBS_USAGESERVICETYPE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +122,25 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4472C4"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4472C4"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -145,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -156,6 +196,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,74 +517,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E234EBB-CE73-4FCB-A4AC-9A74A26E5CDC}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="62.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="62.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="48" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>